<commit_message>
Bajas de alumnos y grupo
Se implementan las bajas para grupos y alumnos, agregando estados para
cada uno (activo [1], inactivo [0]). Se corrije un bug que hacía que
aparecieran grupos repetidos para cambiar de grupo. Se actualizan
plantillas de casos de uso y lista de tareas.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 8va Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 8va Iteración.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\Clon Repo\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA25AC5D-49A4-4346-8C62-C5713DD3AF0C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{798A9300-ECB8-4790-A80C-A222BBA93E51}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -754,7 +754,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="O18" sqref="O18"/>
+      <selection pane="bottomRight" activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1166,102 +1166,104 @@
       <c r="G7" s="5">
         <v>2</v>
       </c>
-      <c r="H7" s="8"/>
+      <c r="H7" s="8">
+        <v>2</v>
+      </c>
       <c r="I7" s="8">
         <f t="shared" ref="I7:I16" si="16">G7-H7</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="8"/>
       <c r="L7" s="8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M7" s="10"/>
       <c r="N7" s="8"/>
       <c r="O7" s="8">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="8"/>
       <c r="R7" s="8">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S7" s="10"/>
       <c r="T7" s="8"/>
       <c r="U7" s="8">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V7" s="10"/>
       <c r="W7" s="8"/>
       <c r="X7" s="8">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y7" s="10"/>
       <c r="Z7" s="8"/>
       <c r="AA7" s="8">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB7" s="10"/>
       <c r="AC7" s="8"/>
       <c r="AD7" s="8">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE7" s="10"/>
       <c r="AF7" s="8"/>
       <c r="AG7" s="8">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AH7" s="10"/>
       <c r="AI7" s="8"/>
       <c r="AJ7" s="8">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AK7" s="10"/>
       <c r="AL7" s="8"/>
       <c r="AM7" s="8">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AN7" s="10"/>
       <c r="AO7" s="8"/>
       <c r="AP7" s="8">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ7" s="10"/>
       <c r="AR7" s="8"/>
       <c r="AS7" s="8">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AT7" s="10"/>
       <c r="AU7" s="8"/>
       <c r="AV7" s="8">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AW7" s="10"/>
       <c r="AX7" s="8"/>
       <c r="AY7" s="8">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AZ7" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA7" s="11">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:53" ht="30" x14ac:dyDescent="0.25">
@@ -1392,102 +1394,104 @@
       <c r="G9" s="5">
         <v>2</v>
       </c>
-      <c r="H9" s="8"/>
+      <c r="H9" s="8">
+        <v>2</v>
+      </c>
       <c r="I9" s="8">
         <f t="shared" si="16"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J9" s="10"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M9" s="10"/>
       <c r="N9" s="8"/>
       <c r="O9" s="8">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P9" s="10"/>
       <c r="Q9" s="8"/>
       <c r="R9" s="8">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S9" s="10"/>
       <c r="T9" s="8"/>
       <c r="U9" s="8">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V9" s="10"/>
       <c r="W9" s="8"/>
       <c r="X9" s="8">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y9" s="10"/>
       <c r="Z9" s="8"/>
       <c r="AA9" s="8">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB9" s="10"/>
       <c r="AC9" s="8"/>
       <c r="AD9" s="8">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE9" s="10"/>
       <c r="AF9" s="8"/>
       <c r="AG9" s="8">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AH9" s="10"/>
       <c r="AI9" s="8"/>
       <c r="AJ9" s="8">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AK9" s="10"/>
       <c r="AL9" s="8"/>
       <c r="AM9" s="8">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AN9" s="10"/>
       <c r="AO9" s="8"/>
       <c r="AP9" s="8">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ9" s="10"/>
       <c r="AR9" s="8"/>
       <c r="AS9" s="8">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AT9" s="10"/>
       <c r="AU9" s="8"/>
       <c r="AV9" s="8">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AW9" s="10"/>
       <c r="AX9" s="8"/>
       <c r="AY9" s="8">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AZ9" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA9" s="11">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:53" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2605,6 +2609,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2616,11 +2625,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Caso de uso consultar registro de asistencias terminado
Se implementa el caso de uso consultar registro de asistencias, se actualizan las plantillas de la iteración.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 8va Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 8va Iteración.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\Clon Repo\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{798A9300-ECB8-4790-A80C-A222BBA93E51}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CAAE348E-942B-4BB2-B773-15DF6AD37455}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -754,7 +754,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="L12" sqref="L12"/>
+      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,96 +1059,98 @@
         <v>3</v>
       </c>
       <c r="J6" s="10"/>
-      <c r="K6" s="8"/>
+      <c r="K6" s="8">
+        <v>4</v>
+      </c>
       <c r="L6" s="8">
         <f t="shared" ref="L6:L16" si="0">I6-K6</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="M6" s="10"/>
       <c r="N6" s="8"/>
       <c r="O6" s="8">
         <f t="shared" ref="O6:O16" si="1">L6-N6</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="8"/>
       <c r="R6" s="8">
         <f t="shared" ref="R6:R16" si="2">O6-Q6</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="S6" s="10"/>
       <c r="T6" s="8"/>
       <c r="U6" s="8">
         <f t="shared" ref="U6:U16" si="3">R6-T6</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="V6" s="10"/>
       <c r="W6" s="8"/>
       <c r="X6" s="8">
         <f t="shared" ref="X6:X16" si="4">U6-W6</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="Y6" s="10"/>
       <c r="Z6" s="8"/>
       <c r="AA6" s="8">
         <f t="shared" ref="AA6:AA16" si="5">X6-Z6</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="AB6" s="10"/>
       <c r="AC6" s="8"/>
       <c r="AD6" s="8">
         <f t="shared" ref="AD6:AD16" si="6">AA6-AC6</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="AE6" s="10"/>
       <c r="AF6" s="8"/>
       <c r="AG6" s="8">
         <f t="shared" ref="AG6:AG16" si="7">AD6-AF6</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="AH6" s="10"/>
       <c r="AI6" s="8"/>
       <c r="AJ6" s="8">
         <f t="shared" ref="AJ6:AJ16" si="8">AG6-AI6</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="AK6" s="10"/>
       <c r="AL6" s="8"/>
       <c r="AM6" s="8">
         <f t="shared" ref="AM6:AM16" si="9">AJ6-AL6</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="AN6" s="10"/>
       <c r="AO6" s="8"/>
       <c r="AP6" s="8">
         <f t="shared" ref="AP6:AP16" si="10">AM6-AO6</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="AQ6" s="10"/>
       <c r="AR6" s="8"/>
       <c r="AS6" s="8">
         <f t="shared" ref="AS6:AS16" si="11">AP6-AR6</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="AT6" s="10"/>
       <c r="AU6" s="8"/>
       <c r="AV6" s="8">
         <f t="shared" ref="AV6:AV16" si="12">AS6-AU6</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="AW6" s="10"/>
       <c r="AX6" s="8"/>
       <c r="AY6" s="8">
         <f t="shared" ref="AY6:AY16" si="13">AV6-AX6</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="AZ6" s="11">
         <f t="shared" ref="AZ6:AZ16" si="14">H6+K6+N6+Q6+T6+W6+Z6+AC6+AF6+AI6+AL6+AO6+AR6+AU6+AX6</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BA6" s="11">
         <f t="shared" ref="BA6:BA16" si="15">G6-AZ6</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="7" spans="2:53" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2609,11 +2611,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2625,6 +2622,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
CU Consultar proximos pagos
Se implementa el CU Consultar proximos pagos (Alumno), se liga un pago a
un grupo, se actualizan plantillas de tareas y casos de uso.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 8va Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 8va Iteración.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CAAE348E-942B-4BB2-B773-15DF6AD37455}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6618C859-0B93-469D-961B-5F6AAB5F9520}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="58">
   <si>
     <t>Columna</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t>Prueba general de sistema en Linux.</t>
+  </si>
+  <si>
+    <t>Hecho</t>
+  </si>
+  <si>
+    <t>En proceso</t>
   </si>
 </sst>
 </file>
@@ -754,7 +760,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1048,7 +1054,7 @@
         <v>40</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="G6" s="5">
         <v>3</v>
@@ -1163,7 +1169,7 @@
         <v>53</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="G7" s="5">
         <v>2</v>
@@ -1278,7 +1284,7 @@
         <v>40</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="G8" s="5">
         <v>3</v>
@@ -1391,7 +1397,7 @@
         <v>53</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="G9" s="5">
         <v>2</v>
@@ -1619,7 +1625,7 @@
         <v>53</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="G11" s="5">
         <v>3</v>
@@ -1630,96 +1636,98 @@
         <v>3</v>
       </c>
       <c r="J11" s="10"/>
-      <c r="K11" s="8"/>
+      <c r="K11" s="8">
+        <v>4</v>
+      </c>
       <c r="L11" s="8">
         <f>I11-K11</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="M11" s="10"/>
       <c r="N11" s="8"/>
       <c r="O11" s="8">
         <f>L11-N11</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="P11" s="10"/>
       <c r="Q11" s="8"/>
       <c r="R11" s="8">
         <f>O11-Q11</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="S11" s="10"/>
       <c r="T11" s="8"/>
       <c r="U11" s="8">
         <f>R11-T11</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="V11" s="10"/>
       <c r="W11" s="8"/>
       <c r="X11" s="8">
         <f>U11-W11</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="Y11" s="10"/>
       <c r="Z11" s="8"/>
       <c r="AA11" s="8">
         <f>X11-Z11</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="AB11" s="10"/>
       <c r="AC11" s="8"/>
       <c r="AD11" s="8">
         <f>AA11-AC11</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="AE11" s="10"/>
       <c r="AF11" s="8"/>
       <c r="AG11" s="8">
         <f>AD11-AF11</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="AH11" s="10"/>
       <c r="AI11" s="8"/>
       <c r="AJ11" s="8">
         <f>AG11-AI11</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="AK11" s="10"/>
       <c r="AL11" s="8"/>
       <c r="AM11" s="8">
         <f>AJ11-AL11</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="AN11" s="10"/>
       <c r="AO11" s="8"/>
       <c r="AP11" s="8">
         <f>AM11-AO11</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="AQ11" s="10"/>
       <c r="AR11" s="8"/>
       <c r="AS11" s="8">
         <f>AP11-AR11</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="AT11" s="10"/>
       <c r="AU11" s="8"/>
       <c r="AV11" s="8">
         <f>AS11-AU11</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="AW11" s="10"/>
       <c r="AX11" s="8"/>
       <c r="AY11" s="8">
         <f>AV11-AX11</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="AZ11" s="11">
         <f>H11+K11+N11+Q11+T11+W11+Z11+AC11+AF11+AI11+AL11+AO11+AR11+AU11+AX11</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BA11" s="11">
         <f>G11-AZ11</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="12" spans="2:53" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Caso de uso consultar proximos pagos profesores terminado.
Se implementa el caso de uso consultar proximos pagos de profesores, se actualiza l plantilla del plan de pruebas y las plantillas de la iteración.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 8va Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 8va Iteración.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6618C859-0B93-469D-961B-5F6AAB5F9520}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CC949B0C-C5A1-4262-A8F1-1FDAC553D05F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="57">
   <si>
     <t>Columna</t>
   </si>
@@ -202,9 +202,6 @@
   </si>
   <si>
     <t>Hecho</t>
-  </si>
-  <si>
-    <t>En proceso</t>
   </si>
 </sst>
 </file>
@@ -760,7 +757,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomRight" activeCell="Z13" sqref="Z13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1284,7 +1281,7 @@
         <v>40</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G8" s="5">
         <v>3</v>
@@ -1301,90 +1298,92 @@
         <v>3</v>
       </c>
       <c r="M8" s="10"/>
-      <c r="N8" s="8"/>
+      <c r="N8" s="8">
+        <v>3</v>
+      </c>
       <c r="O8" s="8">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P8" s="10"/>
       <c r="Q8" s="8"/>
       <c r="R8" s="8">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S8" s="10"/>
       <c r="T8" s="8"/>
       <c r="U8" s="8">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="V8" s="10"/>
       <c r="W8" s="8"/>
       <c r="X8" s="8">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Y8" s="10"/>
       <c r="Z8" s="8"/>
       <c r="AA8" s="8">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AB8" s="10"/>
       <c r="AC8" s="8"/>
       <c r="AD8" s="8">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AE8" s="10"/>
       <c r="AF8" s="8"/>
       <c r="AG8" s="8">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AH8" s="10"/>
       <c r="AI8" s="8"/>
       <c r="AJ8" s="8">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AK8" s="10"/>
       <c r="AL8" s="8"/>
       <c r="AM8" s="8">
         <f t="shared" si="9"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AN8" s="10"/>
       <c r="AO8" s="8"/>
       <c r="AP8" s="8">
         <f t="shared" si="10"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AQ8" s="10"/>
       <c r="AR8" s="8"/>
       <c r="AS8" s="8">
         <f t="shared" si="11"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AT8" s="10"/>
       <c r="AU8" s="8"/>
       <c r="AV8" s="8">
         <f t="shared" si="12"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AW8" s="10"/>
       <c r="AX8" s="8"/>
       <c r="AY8" s="8">
         <f t="shared" si="13"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AZ8" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BA8" s="11">
         <f t="shared" si="15"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:53" ht="45" x14ac:dyDescent="0.25">
@@ -2619,6 +2618,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2630,11 +2634,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización automática del catálogo de alumnos
Se implementa la actualización automática del cat'alogo de alumnos. Se
actualiza la plantilla de tareas.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 8va Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 8va Iteración.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CC949B0C-C5A1-4262-A8F1-1FDAC553D05F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBD89A1-D7FE-4065-85B0-62C9E7897CCE}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -757,7 +757,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="Z13" sqref="Z13"/>
+      <selection pane="bottomRight" activeCell="W11" sqref="W11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1875,84 +1875,86 @@
         <v>4</v>
       </c>
       <c r="P13" s="10"/>
-      <c r="Q13" s="8"/>
+      <c r="Q13" s="8">
+        <v>3</v>
+      </c>
       <c r="R13" s="8">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S13" s="10"/>
       <c r="T13" s="8"/>
       <c r="U13" s="8">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="V13" s="10"/>
       <c r="W13" s="8"/>
       <c r="X13" s="8">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Y13" s="10"/>
       <c r="Z13" s="8"/>
       <c r="AA13" s="8">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AB13" s="10"/>
       <c r="AC13" s="8"/>
       <c r="AD13" s="8">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AE13" s="10"/>
       <c r="AF13" s="8"/>
       <c r="AG13" s="8">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AH13" s="10"/>
       <c r="AI13" s="8"/>
       <c r="AJ13" s="8">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AK13" s="10"/>
       <c r="AL13" s="8"/>
       <c r="AM13" s="8">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AN13" s="10"/>
       <c r="AO13" s="8"/>
       <c r="AP13" s="8">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AQ13" s="10"/>
       <c r="AR13" s="8"/>
       <c r="AS13" s="8">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AT13" s="10"/>
       <c r="AU13" s="8"/>
       <c r="AV13" s="8">
         <f t="shared" si="12"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AW13" s="10"/>
       <c r="AX13" s="8"/>
       <c r="AY13" s="8">
         <f t="shared" si="13"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AZ13" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BA13" s="11">
         <f t="shared" si="15"/>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:53" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2618,11 +2620,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2634,6 +2631,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
cript de base de datos
Se modifica el script de base de datos, se crean correciones del caso de uso consultar proximos pagos de profesor asi como se actualizan las plantillas de la iteración.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 8va Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 8va Iteración.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBD89A1-D7FE-4065-85B0-62C9E7897CCE}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{79D9A000-BCA8-464C-B54B-D9E524BD2F65}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -754,10 +754,10 @@
   <dimension ref="B1:BA19"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="W11" sqref="W11"/>
+      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1511,7 +1511,7 @@
         <v>40</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="G10" s="5">
         <v>2</v>
@@ -1534,84 +1534,86 @@
         <v>3</v>
       </c>
       <c r="P10" s="10"/>
-      <c r="Q10" s="8"/>
+      <c r="Q10" s="8">
+        <v>3</v>
+      </c>
       <c r="R10" s="8">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S10" s="10"/>
       <c r="T10" s="8"/>
       <c r="U10" s="8">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="V10" s="10"/>
       <c r="W10" s="8"/>
       <c r="X10" s="8">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Y10" s="10"/>
       <c r="Z10" s="8"/>
       <c r="AA10" s="8">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AB10" s="10"/>
       <c r="AC10" s="8"/>
       <c r="AD10" s="8">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AE10" s="10"/>
       <c r="AF10" s="8"/>
       <c r="AG10" s="8">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AH10" s="10"/>
       <c r="AI10" s="8"/>
       <c r="AJ10" s="8">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AK10" s="10"/>
       <c r="AL10" s="8"/>
       <c r="AM10" s="8">
         <f t="shared" si="9"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AN10" s="10"/>
       <c r="AO10" s="8"/>
       <c r="AP10" s="8">
         <f t="shared" si="10"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AQ10" s="10"/>
       <c r="AR10" s="8"/>
       <c r="AS10" s="8">
         <f t="shared" si="11"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AT10" s="10"/>
       <c r="AU10" s="8"/>
       <c r="AV10" s="8">
         <f t="shared" si="12"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AW10" s="10"/>
       <c r="AX10" s="8"/>
       <c r="AY10" s="8">
         <f t="shared" si="13"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AZ10" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BA10" s="11">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="11" spans="2:53" ht="48" customHeight="1" x14ac:dyDescent="0.25">
@@ -1762,84 +1764,86 @@
         <v>3</v>
       </c>
       <c r="P12" s="10"/>
-      <c r="Q12" s="8"/>
+      <c r="Q12" s="8">
+        <v>1</v>
+      </c>
       <c r="R12" s="8">
         <f>O12-Q12</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S12" s="10"/>
       <c r="T12" s="8"/>
       <c r="U12" s="8">
         <f>R12-T12</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V12" s="10"/>
       <c r="W12" s="8"/>
       <c r="X12" s="8">
         <f>U12-W12</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Y12" s="10"/>
       <c r="Z12" s="8"/>
       <c r="AA12" s="8">
         <f>X12-Z12</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AB12" s="10"/>
       <c r="AC12" s="8"/>
       <c r="AD12" s="8">
         <f>AA12-AC12</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AE12" s="10"/>
       <c r="AF12" s="8"/>
       <c r="AG12" s="8">
         <f>AD12-AF12</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AH12" s="10"/>
       <c r="AI12" s="8"/>
       <c r="AJ12" s="8">
         <f>AG12-AI12</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AK12" s="10"/>
       <c r="AL12" s="8"/>
       <c r="AM12" s="8">
         <f>AJ12-AL12</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AN12" s="10"/>
       <c r="AO12" s="8"/>
       <c r="AP12" s="8">
         <f>AM12-AO12</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AQ12" s="10"/>
       <c r="AR12" s="8"/>
       <c r="AS12" s="8">
         <f>AP12-AR12</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AT12" s="10"/>
       <c r="AU12" s="8"/>
       <c r="AV12" s="8">
         <f>AS12-AU12</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AW12" s="10"/>
       <c r="AX12" s="8"/>
       <c r="AY12" s="8">
         <f>AV12-AX12</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AZ12" s="11">
         <f>H12+K12+N12+Q12+T12+W12+Z12+AC12+AF12+AI12+AL12+AO12+AR12+AU12+AX12</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA12" s="11">
         <f>G12-AZ12</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="2:53" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2620,6 +2624,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2631,11 +2640,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Instalador de base de datos terminado
Se termina el instalador de base de datos y se implementa la eliminacion
de un registro de renta.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 8va Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 8va Iteración.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
-  <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521189E9-997B-41CA-BCCC-0D6DE2B29CF8}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -21,7 +15,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -210,7 +204,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -454,8 +448,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -753,14 +775,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BA19"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
       <pane xSplit="6" ySplit="5" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="T11" sqref="T11"/>
+      <selection pane="bottomRight" activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1775,78 +1797,80 @@
         <v>2</v>
       </c>
       <c r="S12" s="10"/>
-      <c r="T12" s="8"/>
+      <c r="T12" s="8">
+        <v>4</v>
+      </c>
       <c r="U12" s="8">
         <f>R12-T12</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="V12" s="10"/>
       <c r="W12" s="8"/>
       <c r="X12" s="8">
         <f>U12-W12</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="Y12" s="10"/>
       <c r="Z12" s="8"/>
       <c r="AA12" s="8">
         <f>X12-Z12</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="AB12" s="10"/>
       <c r="AC12" s="8"/>
       <c r="AD12" s="8">
         <f>AA12-AC12</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="AE12" s="10"/>
       <c r="AF12" s="8"/>
       <c r="AG12" s="8">
         <f>AD12-AF12</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="AH12" s="10"/>
       <c r="AI12" s="8"/>
       <c r="AJ12" s="8">
         <f>AG12-AI12</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="AK12" s="10"/>
       <c r="AL12" s="8"/>
       <c r="AM12" s="8">
         <f>AJ12-AL12</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="AN12" s="10"/>
       <c r="AO12" s="8"/>
       <c r="AP12" s="8">
         <f>AM12-AO12</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="AQ12" s="10"/>
       <c r="AR12" s="8"/>
       <c r="AS12" s="8">
         <f>AP12-AR12</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="AT12" s="10"/>
       <c r="AU12" s="8"/>
       <c r="AV12" s="8">
         <f>AS12-AU12</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="AW12" s="10"/>
       <c r="AX12" s="8"/>
       <c r="AY12" s="8">
         <f>AV12-AX12</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="AZ12" s="11">
         <f>H12+K12+N12+Q12+T12+W12+Z12+AC12+AF12+AI12+AL12+AO12+AR12+AU12+AX12</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="BA12" s="11">
         <f>G12-AZ12</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="13" spans="2:53" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2315,7 +2339,7 @@
         <v>54</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G17" s="5">
         <v>1</v>
@@ -2344,78 +2368,80 @@
         <v>1</v>
       </c>
       <c r="S17" s="10"/>
-      <c r="T17" s="8"/>
+      <c r="T17" s="8">
+        <v>3</v>
+      </c>
       <c r="U17" s="8">
         <f t="shared" ref="U17:U19" si="21">R17-T17</f>
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="V17" s="10"/>
       <c r="W17" s="8"/>
       <c r="X17" s="8">
         <f t="shared" ref="X17:X19" si="22">U17-W17</f>
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="Y17" s="10"/>
       <c r="Z17" s="8"/>
       <c r="AA17" s="8">
         <f t="shared" ref="AA17:AA19" si="23">X17-Z17</f>
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="AB17" s="10"/>
       <c r="AC17" s="8"/>
       <c r="AD17" s="8">
         <f t="shared" ref="AD17:AD19" si="24">AA17-AC17</f>
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="AE17" s="10"/>
       <c r="AF17" s="8"/>
       <c r="AG17" s="8">
         <f t="shared" ref="AG17:AG19" si="25">AD17-AF17</f>
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="AH17" s="10"/>
       <c r="AI17" s="8"/>
       <c r="AJ17" s="8">
         <f t="shared" ref="AJ17:AJ19" si="26">AG17-AI17</f>
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="AK17" s="10"/>
       <c r="AL17" s="8"/>
       <c r="AM17" s="8">
         <f t="shared" ref="AM17:AM19" si="27">AJ17-AL17</f>
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="AN17" s="10"/>
       <c r="AO17" s="8"/>
       <c r="AP17" s="8">
         <f t="shared" ref="AP17:AP19" si="28">AM17-AO17</f>
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="AQ17" s="10"/>
       <c r="AR17" s="8"/>
       <c r="AS17" s="8">
         <f t="shared" ref="AS17:AS19" si="29">AP17-AR17</f>
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="AT17" s="10"/>
       <c r="AU17" s="8"/>
       <c r="AV17" s="8">
         <f t="shared" ref="AV17:AV19" si="30">AS17-AU17</f>
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="AW17" s="10"/>
       <c r="AX17" s="8"/>
       <c r="AY17" s="8">
         <f t="shared" ref="AY17:AY19" si="31">AV17-AX17</f>
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="AZ17" s="11">
         <f>H17+K17+N17+Q17+T17+W17+Z17+AC17+AF17+AI17+AL17+AO17+AR17+AU17+AX17</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BA17" s="11">
         <f t="shared" ref="BA17:BA19" si="32">G17-AZ17</f>
-        <v>1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="18" spans="2:53" x14ac:dyDescent="0.25">
@@ -2629,11 +2655,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2645,6 +2666,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2662,7 +2688,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>